<commit_message>
fix filter and chenge SC
</commit_message>
<xml_diff>
--- a/UZ-REPOS/SPA/EDITION/DOC/SCG/Модель услуг SCG v.0.1.xlsx
+++ b/UZ-REPOS/SPA/EDITION/DOC/SCG/Модель услуг SCG v.0.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FORIS_WORK\ SC\UZ\SCG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\@MyRepos\FORIS_WORK\UZ-REPOS\SPA\EDITION\DOC\SCG\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>Версия</t>
   </si>
@@ -126,22 +126,19 @@
     <t>АИИСКУЭ</t>
   </si>
   <si>
-    <t>FRAPABSOLUT</t>
-  </si>
-  <si>
-    <t>Абонентская плата за ТП ABSOLUT</t>
-  </si>
-  <si>
-    <t>FRAPOPTIMA</t>
-  </si>
-  <si>
-    <t>Абонентская плата за ТП Optima</t>
-  </si>
-  <si>
-    <t>Значение параметра 'RFS_SCG_SUBSCRIBER'</t>
-  </si>
-  <si>
-    <t>Значение параметра 'RES_SCG_SUBCRIPTION_TYPE'</t>
+    <t>SCPBREAKSESSION</t>
+  </si>
+  <si>
+    <t>FRINSPECT</t>
+  </si>
+  <si>
+    <t>Разрыв GPRS сессии на SCG</t>
+  </si>
+  <si>
+    <t>Значение параметра 'RES_SCG_PROFILE'</t>
+  </si>
+  <si>
+    <t>Подписка на инспектор</t>
   </si>
 </sst>
 </file>
@@ -316,7 +313,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -429,13 +426,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -449,63 +468,8 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -616,15 +580,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -645,12 +600,49 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color indexed="64"/>
+      <top style="thin">
+        <color rgb="FF000000"/>
       </top>
       <bottom style="medium">
         <color indexed="64"/>
@@ -661,63 +653,28 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -736,7 +693,7 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -799,82 +756,28 @@
     <xf numFmtId="164" fontId="9" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="16" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="6" borderId="18" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="19" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="6" borderId="20" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="6" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -883,28 +786,55 @@
     <xf numFmtId="164" fontId="7" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="29" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="23" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="24" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="25" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="7" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="31" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="19" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="6" borderId="15" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="16" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="6" borderId="17" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="18" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="3" borderId="28" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1321,7 +1251,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="33" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="9" t="s">
@@ -1332,7 +1262,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
+      <c r="A3" s="33"/>
       <c r="B3" s="9" t="s">
         <v>16</v>
       </c>
@@ -1341,7 +1271,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="33" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="9" t="s">
@@ -1352,7 +1282,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
+      <c r="A5" s="33"/>
       <c r="B5" s="9" t="s">
         <v>24</v>
       </c>
@@ -1361,7 +1291,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
+      <c r="A6" s="33"/>
       <c r="B6" s="9" t="s">
         <v>28</v>
       </c>
@@ -1385,7 +1315,7 @@
   <dimension ref="A1:AMN58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1393,10 +1323,10 @@
     <col min="1" max="1" width="13.375" style="15" customWidth="1"/>
     <col min="2" max="2" width="11.25" style="15" customWidth="1"/>
     <col min="3" max="3" width="9.125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="14" style="15" customWidth="1"/>
+    <col min="4" max="4" width="18" style="15" customWidth="1"/>
     <col min="5" max="6" width="14.125" style="15" customWidth="1"/>
     <col min="7" max="7" width="9" style="15" customWidth="1"/>
-    <col min="8" max="8" width="11.875" style="15" customWidth="1"/>
+    <col min="8" max="8" width="17.625" style="15" customWidth="1"/>
     <col min="9" max="9" width="13.5" style="15" customWidth="1"/>
     <col min="10" max="10" width="20.125" style="15" customWidth="1"/>
     <col min="11" max="11" width="16" style="15" customWidth="1"/>
@@ -1408,51 +1338,45 @@
     <col min="17" max="1028" width="8.5" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="43" t="s">
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="23" t="s">
+      <c r="G1" s="40"/>
+      <c r="H1" s="22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="4" customFormat="1" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="34" t="s">
-        <v>39</v>
-      </c>
-      <c r="I2" s="35"/>
-      <c r="J2" s="24"/>
-    </row>
-    <row r="3" spans="1:10" s="4" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="38"/>
+      <c r="H2" s="23"/>
+    </row>
+    <row r="3" spans="1:9" s="4" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>21</v>
       </c>
@@ -1466,50 +1390,46 @@
         <v>34</v>
       </c>
       <c r="E3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="44">
+        <v>0</v>
+      </c>
+      <c r="G3" s="46">
+        <v>1</v>
+      </c>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="1:9" s="4" customFormat="1" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="56">
-        <v>0</v>
-      </c>
-      <c r="G3" s="32">
-        <v>1</v>
-      </c>
-      <c r="H3" s="36"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="24"/>
-    </row>
-    <row r="4" spans="1:10" s="4" customFormat="1" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="51" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="C4" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="49" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="49" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="57"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="24"/>
-    </row>
-    <row r="5" spans="1:10" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="52"/>
-      <c r="B5" s="31" t="s">
+      <c r="E4" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="45"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="23"/>
+    </row>
+    <row r="5" spans="1:9" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="34"/>
+      <c r="B5" s="27" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>16</v>
+      <c r="D5" s="18" t="s">
+        <v>14</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>16</v>
@@ -1520,20 +1440,18 @@
       <c r="G5" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="46"/>
-    </row>
-    <row r="6" spans="1:10" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="53"/>
-      <c r="B6" s="31" t="s">
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="1:9" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="35"/>
+      <c r="B6" s="27" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>16</v>
+      <c r="D6" s="28" t="s">
+        <v>14</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>16</v>
@@ -1544,94 +1462,67 @@
       <c r="G6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="H6" s="40"/>
-      <c r="I6" s="40"/>
-      <c r="J6" s="46"/>
-    </row>
-    <row r="7" spans="1:10" s="4" customFormat="1" ht="18.75" x14ac:dyDescent="0.2">
-      <c r="A7" s="53"/>
-      <c r="B7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="42">
-        <v>111</v>
-      </c>
-      <c r="I7" s="42"/>
-      <c r="J7" s="46"/>
-    </row>
-    <row r="8" spans="1:10" s="4" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="54"/>
-      <c r="B8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" s="42">
-        <v>112</v>
-      </c>
-      <c r="I8" s="42"/>
-      <c r="J8" s="47"/>
-    </row>
-    <row r="9" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="7:11" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="7:11" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="7:11" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="35"/>
+    </row>
+    <row r="8" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="36"/>
+    </row>
+    <row r="9" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I14" s="14"/>
+    </row>
+    <row r="15" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I15" s="14"/>
+    </row>
+    <row r="16" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I16" s="14"/>
+    </row>
+    <row r="17" spans="7:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I17" s="14"/>
+    </row>
+    <row r="18" spans="7:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="I18" s="14"/>
+    </row>
+    <row r="19" spans="7:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+    </row>
     <row r="20" spans="7:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
     </row>
     <row r="21" spans="7:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
     </row>
     <row r="22" spans="7:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
     </row>
     <row r="23" spans="7:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
     </row>
     <row r="24" spans="7:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
     </row>
     <row r="25" spans="7:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
     </row>
@@ -1739,7 +1630,6 @@
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
       <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
       <c r="L37" s="14"/>
@@ -1756,7 +1646,6 @@
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
       <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
       <c r="J38" s="14"/>
       <c r="K38" s="14"/>
       <c r="L38" s="14"/>
@@ -1773,7 +1662,6 @@
       <c r="F39" s="14"/>
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
       <c r="J39" s="14"/>
       <c r="K39" s="14"/>
       <c r="L39" s="14"/>
@@ -1790,7 +1678,6 @@
       <c r="F40" s="14"/>
       <c r="G40" s="14"/>
       <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
       <c r="J40" s="14"/>
       <c r="K40" s="14"/>
       <c r="L40" s="14"/>
@@ -1807,7 +1694,6 @@
       <c r="F41" s="14"/>
       <c r="G41" s="14"/>
       <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
       <c r="J41" s="14"/>
       <c r="K41" s="14"/>
       <c r="L41" s="14"/>
@@ -1824,7 +1710,6 @@
       <c r="F42" s="14"/>
       <c r="G42" s="14"/>
       <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
       <c r="J42" s="14"/>
       <c r="K42" s="14"/>
       <c r="L42" s="14"/>
@@ -1840,8 +1725,6 @@
       <c r="E43" s="14"/>
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
       <c r="J43" s="14"/>
       <c r="K43" s="14"/>
       <c r="L43" s="14"/>
@@ -1857,7 +1740,6 @@
       <c r="E44" s="14"/>
       <c r="F44" s="14"/>
       <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
       <c r="K44" s="14"/>
       <c r="L44" s="14"/>
       <c r="M44" s="14"/>
@@ -1872,7 +1754,6 @@
       <c r="E45" s="14"/>
       <c r="F45" s="14"/>
       <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
       <c r="K45" s="14"/>
       <c r="L45" s="14"/>
       <c r="M45" s="14"/>
@@ -1887,7 +1768,6 @@
       <c r="E46" s="14"/>
       <c r="F46" s="14"/>
       <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
       <c r="K46" s="14"/>
       <c r="L46" s="14"/>
       <c r="M46" s="14"/>
@@ -1902,7 +1782,6 @@
       <c r="E47" s="14"/>
       <c r="F47" s="14"/>
       <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
       <c r="K47" s="14"/>
       <c r="L47" s="14"/>
       <c r="M47" s="14"/>
@@ -1917,7 +1796,6 @@
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
       <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
       <c r="K48" s="14"/>
       <c r="L48" s="14"/>
       <c r="M48" s="14"/>
@@ -1932,7 +1810,6 @@
       <c r="E49" s="14"/>
       <c r="F49" s="14"/>
       <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
       <c r="K49" s="14"/>
       <c r="L49" s="14"/>
       <c r="M49" s="14"/>
@@ -2050,18 +1927,13 @@
       <c r="O58" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A5:A8"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="F1:I1"/>
+  <mergeCells count="6">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="A5:A8"/>
+    <mergeCell ref="F2:G2"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="1.1437007874015745" bottom="1.1437007874015745" header="0.74999999999999989" footer="0.74999999999999989"/>
   <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" horizontalDpi="300" r:id="rId1"/>

</xml_diff>